<commit_message>
List almost complete (needs refactor)
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgomez\IdeaProjects\ApiTraining\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgomez\IdeaProjects\TheMovieDBApiTesting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269056A-D817-4160-BCC9-F69A26810596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3837B1-615F-4CAB-A38B-4B0481ED0D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
     <sheet name="Movies" sheetId="4" r:id="rId4"/>
+    <sheet name="ListDetails" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -94,19 +95,37 @@
   </si>
   <si>
     <t>FamiliaList</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>created by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,13 +440,13 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -452,12 +475,12 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -473,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -490,18 +513,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8E1107-5E6B-4146-A655-33CEBE14901F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -512,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -523,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -534,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -559,9 +582,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -569,7 +592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -577,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -588,4 +611,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A24B17-723D-45B7-8D59-FC1E57F0533E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>7105904</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All test cases done
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgomez\IdeaProjects\TheMovieDBApiTesting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E8E060-93DA-450B-AEA5-8D541BABD401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0070A3-E27E-494F-BD1B-CB5286A864A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="27015" windowHeight="14010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="27015" windowHeight="14010" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidCredentials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>username</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>matrix</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>terror</t>
@@ -571,10 +568,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -582,10 +579,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -601,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758B04FE-B548-4D62-993E-F74015ED93EA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,10 +621,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -635,10 +632,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -677,10 +674,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -688,10 +685,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -704,36 +701,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0D3EEB-4820-40B5-BE80-045BABB739CF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -756,13 +744,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -794,10 +782,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,10 +816,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>